<commit_message>
finalized data and edits for thesis
</commit_message>
<xml_diff>
--- a/moreanalysis.xlsx
+++ b/moreanalysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wesley\Documents\GitHub\Modelling-Disease-with-Twitter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wesley\Documents\GitHub\Modeling-Disease-with-Twitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9968"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9968" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="tobiData" sheetId="14" r:id="rId1"/>
@@ -1195,11 +1195,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="440839504"/>
-        <c:axId val="440840288"/>
+        <c:axId val="713120944"/>
+        <c:axId val="713119376"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="440839504"/>
+        <c:axId val="713120944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,14 +1242,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440840288"/>
+        <c:crossAx val="713119376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="440840288"/>
+        <c:axId val="713119376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1300,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440839504"/>
+        <c:crossAx val="713120944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2900,11 +2900,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="440841072"/>
-        <c:axId val="481263488"/>
+        <c:axId val="713119768"/>
+        <c:axId val="713118592"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="440841072"/>
+        <c:axId val="713119768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2947,14 +2947,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481263488"/>
+        <c:crossAx val="713118592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="481263488"/>
+        <c:axId val="713118592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3005,7 +3005,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440841072"/>
+        <c:crossAx val="713119768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4636,11 +4636,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="481274856"/>
-        <c:axId val="481272112"/>
+        <c:axId val="713120552"/>
+        <c:axId val="713120160"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="481274856"/>
+        <c:axId val="713120552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4683,14 +4683,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481272112"/>
+        <c:crossAx val="713120160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="481272112"/>
+        <c:axId val="713120160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4741,7 +4741,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481274856"/>
+        <c:crossAx val="713120552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6864,8 +6864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T2" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:AM28"/>
+    <sheetView topLeftCell="AF14" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15697,8 +15697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:U28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18526,7 +18526,7 @@
         <v>0.85870531949436413</v>
       </c>
       <c r="X30">
-        <f t="shared" si="24"/>
+        <f>CORREL(X2:X19,$Z$2:$Z$19)</f>
         <v>0.86475292951832972</v>
       </c>
       <c r="Y30">

</xml_diff>